<commit_message>
logs limpos, downloads corretos e etl base, e recebido ok
</commit_message>
<xml_diff>
--- a/downloads/ControleODONTO Fluxo de Caixa (2).xlsx
+++ b/downloads/ControleODONTO Fluxo de Caixa (2).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4048" uniqueCount="4048">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="4187">
   <x:si>
     <x:t>Data</x:t>
   </x:si>
@@ -12151,22 +12151,439 @@
     <x:t>6.335,00</x:t>
   </x:si>
   <x:si>
+    <x:t>014010 1/5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.492,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10,47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11935500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7214</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maria Raimunda Pinheiro dos Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>656.014.085-72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014011 1/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27410</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alessandra Lima Pereira</x:t>
+  </x:si>
+  <x:si>
+    <x:t>135.181.627-64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>012896 1/1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>877,50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paciente não se adaptou com o aparelho Estético lançado no contrato 11620 pediu para alterar para o convencional, pois disse que achou muito estranho gerado título para troca da diferença entre os tipos de aparelho, utilizado saldo restante para remoção e aparelho móvel, finaceiro ciente dado baixa como estorno de pagamento.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5887</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Letícia Nascimento dos Reis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>858.879.855-77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>011887 4/10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Não paga manutenção do fixo!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Antonia Vania Oliveira Batista</x:t>
+  </x:si>
+  <x:si>
+    <x:t>010.129.025-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>012555 4/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>159,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26692</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paulino José dos Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>117.394.955-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>010055 10/18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>966,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2948</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Emilly Vieira da Silva</x:t>
+  </x:si>
+  <x:si>
+    <x:t>114.072.415-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>010235 9/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zirlande Augusta Lima de Sant'anna</x:t>
+  </x:si>
+  <x:si>
+    <x:t>896.567.255-49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>010774 7/19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>966,67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7258</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maria Telma Santos do Nascimento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>641.353.495-87</x:t>
+  </x:si>
+  <x:si>
+    <x:t>011831 4/9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26289</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rosiel dos Santos Oliveira</x:t>
+  </x:si>
+  <x:si>
+    <x:t>687.513.705-49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>009286 10/31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>732,70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25622</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alexsandro Almeida de Jesus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014.652.005-09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>007949 14/25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>822,07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28126</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caroline Lemos de Santana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>463.193.875-72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014013 1/1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28/08/2025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014014 1/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014014 2/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16,53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>273271</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8890</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robson Ferreira Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>862.547.625-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014016 1/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24513</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maria da Conceição DOS Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>582.927.805-72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>006066 31/31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/10/2026</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24388</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jonathan Felipe Farias DOS Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>079.168.275-73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014018 1/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23224</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vanessa Santos Auto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>067.532.665-69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>009408 9/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20/08/2025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8451</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rafhaella Silva Nascimento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>046.317.105-51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013747 1/18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>774959</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26832</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jefferson Santos Costa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>883.115.975-53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013552 1/8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>905,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16388888</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23108</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mariene Galdino Rodrigues Sousa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>086.356.765-72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>012694 4/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vanine Meneses PJ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013552 1/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ANTÔNIO PEDIU PARA DA BAIXA A DIFERENÇA DO VALOR COMO CORTESIA. DIFERENÇA DO APARELHO MÓVEL.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013552 2/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014012 1/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16504878</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27664</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alex da Silva Pacheco</x:t>
+  </x:si>
+  <x:si>
+    <x:t>958.835.845-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013664 2/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24/10/2025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paciente foi beneficiado com uma manutenção gratuita pela indicação Rosilene de Souza Oliveira, paciente ciente</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10208</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vanuza Matos Almeida</x:t>
+  </x:si>
+  <x:si>
+    <x:t>899.803.365-87</x:t>
+  </x:si>
+  <x:si>
+    <x:t>012972 3/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>273274</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3341</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flávia Silva Nunes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>025.641.895-04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013394 2/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Transferência Bancária</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013963 1/32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24051</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raniere Bomfim Souza Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>794.008.335-04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014019 1/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.799,00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20533735</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jessica Alves</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26585</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Italo Gabriel Souza Santana Santos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>097.595.075-44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>014020 1/1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23669</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sophia Menezes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>073.867.235-12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>013509 2/12</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Marschall Induatria Comercio Importação </x:t>
+  </x:si>
+  <x:si>
     <x:t>Total</x:t>
   </x:si>
   <x:si>
-    <x:t>775.551,64</x:t>
-  </x:si>
-  <x:si>
-    <x:t>684.846,36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.348,23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>203,25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6.270,44</x:t>
+    <x:t>794.926,58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>704.011,80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.389,53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>211,75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6.433,44</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -12276,8 +12693,8 @@
 </file>
 
 <file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AC855" totalsRowShown="0">
-  <x:autoFilter ref="A1:AC855"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AC886" totalsRowShown="0">
+  <x:autoFilter ref="A1:AC886"/>
   <x:tableColumns count="29">
     <x:tableColumn id="1" name="Data"/>
     <x:tableColumn id="2" name="Transação"/>
@@ -12601,7 +13018,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AC855"/>
+  <x:dimension ref="A1:AC886"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -73464,84 +73881,2297 @@
       <x:c r="AC853" s="0" t="s"/>
     </x:row>
     <x:row r="854" spans="1:29">
-      <x:c r="A854" s="0" t="s"/>
-      <x:c r="B854" s="0" t="s"/>
-      <x:c r="C854" s="0" t="s"/>
-      <x:c r="D854" s="0" t="s"/>
-      <x:c r="E854" s="0" t="s"/>
-      <x:c r="F854" s="0" t="s"/>
-      <x:c r="G854" s="0" t="s"/>
-      <x:c r="H854" s="0" t="s"/>
-      <x:c r="I854" s="0" t="s"/>
-      <x:c r="J854" s="0" t="s"/>
-      <x:c r="K854" s="0" t="s"/>
-      <x:c r="L854" s="0" t="s"/>
-      <x:c r="M854" s="0" t="s"/>
-      <x:c r="N854" s="0" t="s"/>
+      <x:c r="A854" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B854" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C854" s="0" t="s">
+        <x:v>4030</x:v>
+      </x:c>
+      <x:c r="D854" s="0" t="s">
+        <x:v>4031</x:v>
+      </x:c>
+      <x:c r="E854" s="0" t="s">
+        <x:v>4032</x:v>
+      </x:c>
+      <x:c r="F854" s="0" t="s">
+        <x:v>4042</x:v>
+      </x:c>
+      <x:c r="G854" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="H854" s="1" t="s">
+        <x:v>4043</x:v>
+      </x:c>
+      <x:c r="I854" s="2" t="s">
+        <x:v>4043</x:v>
+      </x:c>
+      <x:c r="J854" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K854" s="3" t="s">
+        <x:v>4043</x:v>
+      </x:c>
+      <x:c r="L854" s="0" t="s">
+        <x:v>4044</x:v>
+      </x:c>
+      <x:c r="M854" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N854" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
       <x:c r="O854" s="0" t="s"/>
       <x:c r="P854" s="0" t="s"/>
-      <x:c r="Q854" s="0" t="s"/>
-      <x:c r="R854" s="0" t="s"/>
-      <x:c r="S854" s="0" t="s"/>
-      <x:c r="T854" s="0" t="s"/>
-      <x:c r="U854" s="0" t="s"/>
-      <x:c r="V854" s="0" t="s"/>
-      <x:c r="W854" s="0" t="s"/>
+      <x:c r="Q854" s="0" t="s">
+        <x:v>732</x:v>
+      </x:c>
+      <x:c r="R854" s="0" t="s">
+        <x:v>4045</x:v>
+      </x:c>
+      <x:c r="S854" s="0" t="s">
+        <x:v>3968</x:v>
+      </x:c>
+      <x:c r="T854" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="U854" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="V854" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="W854" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
       <x:c r="X854" s="0" t="s"/>
       <x:c r="Y854" s="0" t="s"/>
       <x:c r="Z854" s="0" t="s"/>
       <x:c r="AA854" s="0" t="s"/>
-      <x:c r="AB854" s="0" t="s"/>
+      <x:c r="AB854" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
       <x:c r="AC854" s="0" t="s"/>
     </x:row>
     <x:row r="855" spans="1:29">
-      <x:c r="A855" s="0" t="s"/>
-      <x:c r="B855" s="0" t="s"/>
-      <x:c r="C855" s="0" t="s"/>
+      <x:c r="A855" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B855" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C855" s="0" t="s">
+        <x:v>4046</x:v>
+      </x:c>
       <x:c r="D855" s="0" t="s">
-        <x:v>4042</x:v>
-      </x:c>
-      <x:c r="E855" s="0" t="s"/>
-      <x:c r="F855" s="0" t="s"/>
-      <x:c r="G855" s="0" t="s"/>
-      <x:c r="H855" s="0" t="s">
-        <x:v>4043</x:v>
-      </x:c>
-      <x:c r="I855" s="0" t="s">
-        <x:v>4044</x:v>
+        <x:v>4047</x:v>
+      </x:c>
+      <x:c r="E855" s="0" t="s">
+        <x:v>4048</x:v>
+      </x:c>
+      <x:c r="F855" s="0" t="s">
+        <x:v>4049</x:v>
+      </x:c>
+      <x:c r="G855" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H855" s="1" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="I855" s="2" t="s">
+        <x:v>167</x:v>
       </x:c>
       <x:c r="J855" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="K855" s="0" t="s"/>
+      <x:c r="K855" s="3" t="s">
+        <x:v>167</x:v>
+      </x:c>
       <x:c r="L855" s="0" t="s">
-        <x:v>4045</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M855" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
       <x:c r="N855" s="0" t="s">
-        <x:v>4046</x:v>
-      </x:c>
-      <x:c r="O855" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="P855" s="0" t="s">
-        <x:v>4047</x:v>
-      </x:c>
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O855" s="0" t="s"/>
+      <x:c r="P855" s="0" t="s"/>
       <x:c r="Q855" s="0" t="s"/>
       <x:c r="R855" s="0" t="s"/>
       <x:c r="S855" s="0" t="s"/>
-      <x:c r="T855" s="0" t="s"/>
-      <x:c r="U855" s="0" t="s"/>
-      <x:c r="V855" s="0" t="s"/>
-      <x:c r="W855" s="0" t="s"/>
+      <x:c r="T855" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U855" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="V855" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="W855" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
       <x:c r="X855" s="0" t="s"/>
-      <x:c r="Y855" s="0" t="s"/>
+      <x:c r="Y855" s="0" t="s">
+        <x:v>646</x:v>
+      </x:c>
       <x:c r="Z855" s="0" t="s"/>
       <x:c r="AA855" s="0" t="s"/>
-      <x:c r="AB855" s="0" t="s"/>
+      <x:c r="AB855" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
       <x:c r="AC855" s="0" t="s"/>
+    </x:row>
+    <x:row r="856" spans="1:29">
+      <x:c r="A856" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B856" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C856" s="0" t="s">
+        <x:v>4050</x:v>
+      </x:c>
+      <x:c r="D856" s="0" t="s">
+        <x:v>4051</x:v>
+      </x:c>
+      <x:c r="E856" s="0" t="s">
+        <x:v>4052</x:v>
+      </x:c>
+      <x:c r="F856" s="0" t="s">
+        <x:v>4053</x:v>
+      </x:c>
+      <x:c r="G856" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H856" s="1" t="s">
+        <x:v>4054</x:v>
+      </x:c>
+      <x:c r="I856" s="2" t="s">
+        <x:v>4054</x:v>
+      </x:c>
+      <x:c r="J856" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K856" s="3" t="s">
+        <x:v>4054</x:v>
+      </x:c>
+      <x:c r="L856" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M856" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N856" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O856" s="0" t="s"/>
+      <x:c r="P856" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q856" s="0" t="s"/>
+      <x:c r="R856" s="0" t="s"/>
+      <x:c r="S856" s="0" t="s"/>
+      <x:c r="T856" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U856" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="V856" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W856" s="0" t="s">
+        <x:v>3698</x:v>
+      </x:c>
+      <x:c r="X856" s="0" t="s"/>
+      <x:c r="Y856" s="0" t="s">
+        <x:v>4055</x:v>
+      </x:c>
+      <x:c r="Z856" s="0" t="s"/>
+      <x:c r="AA856" s="0" t="s"/>
+      <x:c r="AB856" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC856" s="0" t="s"/>
+    </x:row>
+    <x:row r="857" spans="1:29">
+      <x:c r="A857" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B857" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C857" s="0" t="s">
+        <x:v>4056</x:v>
+      </x:c>
+      <x:c r="D857" s="0" t="s">
+        <x:v>4057</x:v>
+      </x:c>
+      <x:c r="E857" s="0" t="s">
+        <x:v>4058</x:v>
+      </x:c>
+      <x:c r="F857" s="0" t="s">
+        <x:v>4059</x:v>
+      </x:c>
+      <x:c r="G857" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H857" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="I857" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="J857" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K857" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="L857" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M857" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N857" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O857" s="0" t="s"/>
+      <x:c r="P857" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q857" s="0" t="s"/>
+      <x:c r="R857" s="0" t="s"/>
+      <x:c r="S857" s="0" t="s"/>
+      <x:c r="T857" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U857" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V857" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W857" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="X857" s="0" t="s"/>
+      <x:c r="Y857" s="0" t="s">
+        <x:v>4060</x:v>
+      </x:c>
+      <x:c r="Z857" s="0" t="s"/>
+      <x:c r="AA857" s="0" t="s"/>
+      <x:c r="AB857" s="0" t="s"/>
+      <x:c r="AC857" s="0" t="s"/>
+    </x:row>
+    <x:row r="858" spans="1:29">
+      <x:c r="A858" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B858" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C858" s="0" t="s">
+        <x:v>4061</x:v>
+      </x:c>
+      <x:c r="D858" s="0" t="s">
+        <x:v>4062</x:v>
+      </x:c>
+      <x:c r="E858" s="0" t="s">
+        <x:v>4063</x:v>
+      </x:c>
+      <x:c r="F858" s="0" t="s">
+        <x:v>4064</x:v>
+      </x:c>
+      <x:c r="G858" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H858" s="1" t="s">
+        <x:v>4065</x:v>
+      </x:c>
+      <x:c r="I858" s="2" t="s">
+        <x:v>3690</x:v>
+      </x:c>
+      <x:c r="J858" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K858" s="3" t="s">
+        <x:v>3690</x:v>
+      </x:c>
+      <x:c r="L858" s="0" t="s"/>
+      <x:c r="M858" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N858" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O858" s="0" t="s"/>
+      <x:c r="P858" s="0" t="s">
+        <x:v>4066</x:v>
+      </x:c>
+      <x:c r="Q858" s="0" t="s"/>
+      <x:c r="R858" s="0" t="s"/>
+      <x:c r="S858" s="0" t="s"/>
+      <x:c r="T858" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U858" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V858" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W858" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="X858" s="0" t="s"/>
+      <x:c r="Y858" s="0" t="s"/>
+      <x:c r="Z858" s="0" t="s"/>
+      <x:c r="AA858" s="0" t="s"/>
+      <x:c r="AB858" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC858" s="0" t="s"/>
+    </x:row>
+    <x:row r="859" spans="1:29">
+      <x:c r="A859" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B859" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C859" s="0" t="s">
+        <x:v>4067</x:v>
+      </x:c>
+      <x:c r="D859" s="0" t="s">
+        <x:v>4068</x:v>
+      </x:c>
+      <x:c r="E859" s="0" t="s">
+        <x:v>4069</x:v>
+      </x:c>
+      <x:c r="F859" s="0" t="s">
+        <x:v>4070</x:v>
+      </x:c>
+      <x:c r="G859" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H859" s="1" t="s">
+        <x:v>4071</x:v>
+      </x:c>
+      <x:c r="I859" s="2" t="s">
+        <x:v>4071</x:v>
+      </x:c>
+      <x:c r="J859" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K859" s="3" t="s">
+        <x:v>4071</x:v>
+      </x:c>
+      <x:c r="L859" s="0" t="s"/>
+      <x:c r="M859" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N859" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O859" s="0" t="s"/>
+      <x:c r="P859" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q859" s="0" t="s"/>
+      <x:c r="R859" s="0" t="s"/>
+      <x:c r="S859" s="0" t="s"/>
+      <x:c r="T859" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U859" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="V859" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W859" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X859" s="0" t="s"/>
+      <x:c r="Y859" s="0" t="s"/>
+      <x:c r="Z859" s="0" t="s"/>
+      <x:c r="AA859" s="0" t="s"/>
+      <x:c r="AB859" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC859" s="0" t="s"/>
+    </x:row>
+    <x:row r="860" spans="1:29">
+      <x:c r="A860" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B860" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C860" s="0" t="s">
+        <x:v>4072</x:v>
+      </x:c>
+      <x:c r="D860" s="0" t="s">
+        <x:v>4073</x:v>
+      </x:c>
+      <x:c r="E860" s="0" t="s">
+        <x:v>4074</x:v>
+      </x:c>
+      <x:c r="F860" s="0" t="s">
+        <x:v>4075</x:v>
+      </x:c>
+      <x:c r="G860" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H860" s="1" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="I860" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J860" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K860" s="3" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="L860" s="0" t="s"/>
+      <x:c r="M860" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N860" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O860" s="0" t="s"/>
+      <x:c r="P860" s="0" t="s"/>
+      <x:c r="Q860" s="0" t="s"/>
+      <x:c r="R860" s="0" t="s"/>
+      <x:c r="S860" s="0" t="s"/>
+      <x:c r="T860" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U860" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V860" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W860" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="X860" s="0" t="s"/>
+      <x:c r="Y860" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z860" s="0" t="s">
+        <x:v>3470</x:v>
+      </x:c>
+      <x:c r="AA860" s="0" t="s">
+        <x:v>3471</x:v>
+      </x:c>
+      <x:c r="AB860" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="AC860" s="0" t="s"/>
+    </x:row>
+    <x:row r="861" spans="1:29">
+      <x:c r="A861" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B861" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C861" s="0" t="s">
+        <x:v>4076</x:v>
+      </x:c>
+      <x:c r="D861" s="0" t="s">
+        <x:v>4077</x:v>
+      </x:c>
+      <x:c r="E861" s="0" t="s">
+        <x:v>4078</x:v>
+      </x:c>
+      <x:c r="F861" s="0" t="s">
+        <x:v>4079</x:v>
+      </x:c>
+      <x:c r="G861" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H861" s="1" t="s">
+        <x:v>4080</x:v>
+      </x:c>
+      <x:c r="I861" s="2" t="s">
+        <x:v>4080</x:v>
+      </x:c>
+      <x:c r="J861" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K861" s="3" t="s">
+        <x:v>4080</x:v>
+      </x:c>
+      <x:c r="L861" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M861" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N861" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O861" s="0" t="s"/>
+      <x:c r="P861" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q861" s="0" t="s"/>
+      <x:c r="R861" s="0" t="s"/>
+      <x:c r="S861" s="0" t="s"/>
+      <x:c r="T861" s="0" t="s">
+        <x:v>2146</x:v>
+      </x:c>
+      <x:c r="U861" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="V861" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W861" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="X861" s="0" t="s"/>
+      <x:c r="Y861" s="0" t="s">
+        <x:v>2644</x:v>
+      </x:c>
+      <x:c r="Z861" s="0" t="s"/>
+      <x:c r="AA861" s="0" t="s"/>
+      <x:c r="AB861" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC861" s="0" t="s"/>
+    </x:row>
+    <x:row r="862" spans="1:29">
+      <x:c r="A862" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B862" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C862" s="0" t="s">
+        <x:v>4081</x:v>
+      </x:c>
+      <x:c r="D862" s="0" t="s">
+        <x:v>4082</x:v>
+      </x:c>
+      <x:c r="E862" s="0" t="s">
+        <x:v>4083</x:v>
+      </x:c>
+      <x:c r="F862" s="0" t="s">
+        <x:v>4084</x:v>
+      </x:c>
+      <x:c r="G862" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H862" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="I862" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="J862" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K862" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="L862" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M862" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N862" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O862" s="0" t="s"/>
+      <x:c r="P862" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q862" s="0" t="s"/>
+      <x:c r="R862" s="0" t="s"/>
+      <x:c r="S862" s="0" t="s"/>
+      <x:c r="T862" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U862" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V862" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W862" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="X862" s="0" t="s"/>
+      <x:c r="Y862" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="Z862" s="0" t="s"/>
+      <x:c r="AA862" s="0" t="s"/>
+      <x:c r="AB862" s="0" t="s"/>
+      <x:c r="AC862" s="0" t="s"/>
+    </x:row>
+    <x:row r="863" spans="1:29">
+      <x:c r="A863" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B863" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C863" s="0" t="s">
+        <x:v>4085</x:v>
+      </x:c>
+      <x:c r="D863" s="0" t="s">
+        <x:v>4086</x:v>
+      </x:c>
+      <x:c r="E863" s="0" t="s">
+        <x:v>4087</x:v>
+      </x:c>
+      <x:c r="F863" s="0" t="s">
+        <x:v>4088</x:v>
+      </x:c>
+      <x:c r="G863" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H863" s="1" t="s">
+        <x:v>4089</x:v>
+      </x:c>
+      <x:c r="I863" s="2" t="s">
+        <x:v>4089</x:v>
+      </x:c>
+      <x:c r="J863" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K863" s="3" t="s">
+        <x:v>4089</x:v>
+      </x:c>
+      <x:c r="L863" s="0" t="s"/>
+      <x:c r="M863" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N863" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O863" s="0" t="s"/>
+      <x:c r="P863" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q863" s="0" t="s"/>
+      <x:c r="R863" s="0" t="s"/>
+      <x:c r="S863" s="0" t="s"/>
+      <x:c r="T863" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U863" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="V863" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="W863" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="X863" s="0" t="s"/>
+      <x:c r="Y863" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z863" s="0" t="s"/>
+      <x:c r="AA863" s="0" t="s"/>
+      <x:c r="AB863" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC863" s="0" t="s"/>
+    </x:row>
+    <x:row r="864" spans="1:29">
+      <x:c r="A864" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B864" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C864" s="0" t="s">
+        <x:v>4090</x:v>
+      </x:c>
+      <x:c r="D864" s="0" t="s">
+        <x:v>4091</x:v>
+      </x:c>
+      <x:c r="E864" s="0" t="s">
+        <x:v>4092</x:v>
+      </x:c>
+      <x:c r="F864" s="0" t="s">
+        <x:v>4093</x:v>
+      </x:c>
+      <x:c r="G864" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H864" s="1" t="s">
+        <x:v>4094</x:v>
+      </x:c>
+      <x:c r="I864" s="2" t="s">
+        <x:v>4094</x:v>
+      </x:c>
+      <x:c r="J864" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K864" s="3" t="s">
+        <x:v>4094</x:v>
+      </x:c>
+      <x:c r="L864" s="0" t="s"/>
+      <x:c r="M864" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N864" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O864" s="0" t="s"/>
+      <x:c r="P864" s="0" t="s"/>
+      <x:c r="Q864" s="0" t="s"/>
+      <x:c r="R864" s="0" t="s"/>
+      <x:c r="S864" s="0" t="s"/>
+      <x:c r="T864" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U864" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="V864" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W864" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X864" s="0" t="s"/>
+      <x:c r="Y864" s="0" t="s">
+        <x:v>3807</x:v>
+      </x:c>
+      <x:c r="Z864" s="0" t="s"/>
+      <x:c r="AA864" s="0" t="s"/>
+      <x:c r="AB864" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC864" s="0" t="s"/>
+    </x:row>
+    <x:row r="865" spans="1:29">
+      <x:c r="A865" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B865" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C865" s="0" t="s">
+        <x:v>4095</x:v>
+      </x:c>
+      <x:c r="D865" s="0" t="s">
+        <x:v>4096</x:v>
+      </x:c>
+      <x:c r="E865" s="0" t="s">
+        <x:v>4097</x:v>
+      </x:c>
+      <x:c r="F865" s="0" t="s">
+        <x:v>4098</x:v>
+      </x:c>
+      <x:c r="G865" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H865" s="1" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="I865" s="2" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="J865" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K865" s="3" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="L865" s="0" t="s"/>
+      <x:c r="M865" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N865" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O865" s="0" t="s"/>
+      <x:c r="P865" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q865" s="0" t="s"/>
+      <x:c r="R865" s="0" t="s"/>
+      <x:c r="S865" s="0" t="s"/>
+      <x:c r="T865" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U865" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V865" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="W865" s="0" t="s">
+        <x:v>4099</x:v>
+      </x:c>
+      <x:c r="X865" s="0" t="s"/>
+      <x:c r="Y865" s="0" t="s"/>
+      <x:c r="Z865" s="0" t="s"/>
+      <x:c r="AA865" s="0" t="s"/>
+      <x:c r="AB865" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC865" s="0" t="s"/>
+    </x:row>
+    <x:row r="866" spans="1:29">
+      <x:c r="A866" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B866" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C866" s="0" t="s">
+        <x:v>4095</x:v>
+      </x:c>
+      <x:c r="D866" s="0" t="s">
+        <x:v>4096</x:v>
+      </x:c>
+      <x:c r="E866" s="0" t="s">
+        <x:v>4097</x:v>
+      </x:c>
+      <x:c r="F866" s="0" t="s">
+        <x:v>4100</x:v>
+      </x:c>
+      <x:c r="G866" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H866" s="1" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="I866" s="2" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="J866" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K866" s="3" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="L866" s="0" t="s"/>
+      <x:c r="M866" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N866" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O866" s="0" t="s"/>
+      <x:c r="P866" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q866" s="0" t="s"/>
+      <x:c r="R866" s="0" t="s"/>
+      <x:c r="S866" s="0" t="s"/>
+      <x:c r="T866" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U866" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V866" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="W866" s="0" t="s">
+        <x:v>4099</x:v>
+      </x:c>
+      <x:c r="X866" s="0" t="s"/>
+      <x:c r="Y866" s="0" t="s"/>
+      <x:c r="Z866" s="0" t="s"/>
+      <x:c r="AA866" s="0" t="s"/>
+      <x:c r="AB866" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC866" s="0" t="s"/>
+    </x:row>
+    <x:row r="867" spans="1:29">
+      <x:c r="A867" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B867" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C867" s="0" t="s">
+        <x:v>4095</x:v>
+      </x:c>
+      <x:c r="D867" s="0" t="s">
+        <x:v>4096</x:v>
+      </x:c>
+      <x:c r="E867" s="0" t="s">
+        <x:v>4097</x:v>
+      </x:c>
+      <x:c r="F867" s="0" t="s">
+        <x:v>4101</x:v>
+      </x:c>
+      <x:c r="G867" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="H867" s="1" t="s">
+        <x:v>1784</x:v>
+      </x:c>
+      <x:c r="I867" s="2" t="s">
+        <x:v>1784</x:v>
+      </x:c>
+      <x:c r="J867" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K867" s="3" t="s">
+        <x:v>1784</x:v>
+      </x:c>
+      <x:c r="L867" s="0" t="s">
+        <x:v>4102</x:v>
+      </x:c>
+      <x:c r="M867" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N867" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O867" s="0" t="s"/>
+      <x:c r="P867" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q867" s="0" t="s"/>
+      <x:c r="R867" s="0" t="s">
+        <x:v>4103</x:v>
+      </x:c>
+      <x:c r="S867" s="0" t="s"/>
+      <x:c r="T867" s="0" t="s">
+        <x:v>3911</x:v>
+      </x:c>
+      <x:c r="U867" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V867" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="W867" s="0" t="s">
+        <x:v>764</x:v>
+      </x:c>
+      <x:c r="X867" s="0" t="s"/>
+      <x:c r="Y867" s="0" t="s"/>
+      <x:c r="Z867" s="0" t="s"/>
+      <x:c r="AA867" s="0" t="s"/>
+      <x:c r="AB867" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC867" s="0" t="s"/>
+    </x:row>
+    <x:row r="868" spans="1:29">
+      <x:c r="A868" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B868" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C868" s="0" t="s">
+        <x:v>4104</x:v>
+      </x:c>
+      <x:c r="D868" s="0" t="s">
+        <x:v>4105</x:v>
+      </x:c>
+      <x:c r="E868" s="0" t="s">
+        <x:v>4106</x:v>
+      </x:c>
+      <x:c r="F868" s="0" t="s">
+        <x:v>4107</x:v>
+      </x:c>
+      <x:c r="G868" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H868" s="1" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="I868" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J868" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K868" s="3" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="L868" s="0" t="s"/>
+      <x:c r="M868" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N868" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O868" s="0" t="s"/>
+      <x:c r="P868" s="0" t="s"/>
+      <x:c r="Q868" s="0" t="s"/>
+      <x:c r="R868" s="0" t="s"/>
+      <x:c r="S868" s="0" t="s"/>
+      <x:c r="T868" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U868" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V868" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W868" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X868" s="0" t="s"/>
+      <x:c r="Y868" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z868" s="0" t="s"/>
+      <x:c r="AA868" s="0" t="s"/>
+      <x:c r="AB868" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC868" s="0" t="s"/>
+    </x:row>
+    <x:row r="869" spans="1:29">
+      <x:c r="A869" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B869" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C869" s="0" t="s">
+        <x:v>4108</x:v>
+      </x:c>
+      <x:c r="D869" s="0" t="s">
+        <x:v>4109</x:v>
+      </x:c>
+      <x:c r="E869" s="0" t="s">
+        <x:v>4110</x:v>
+      </x:c>
+      <x:c r="F869" s="0" t="s">
+        <x:v>4111</x:v>
+      </x:c>
+      <x:c r="G869" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H869" s="1" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="I869" s="2" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="J869" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K869" s="3" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="L869" s="0" t="s"/>
+      <x:c r="M869" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N869" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O869" s="0" t="s"/>
+      <x:c r="P869" s="0" t="s"/>
+      <x:c r="Q869" s="0" t="s"/>
+      <x:c r="R869" s="0" t="s"/>
+      <x:c r="S869" s="0" t="s"/>
+      <x:c r="T869" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U869" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="V869" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W869" s="0" t="s">
+        <x:v>4112</x:v>
+      </x:c>
+      <x:c r="X869" s="0" t="s"/>
+      <x:c r="Y869" s="0" t="s"/>
+      <x:c r="Z869" s="0" t="s"/>
+      <x:c r="AA869" s="0" t="s"/>
+      <x:c r="AB869" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC869" s="0" t="s"/>
+    </x:row>
+    <x:row r="870" spans="1:29">
+      <x:c r="A870" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B870" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C870" s="0" t="s">
+        <x:v>4113</x:v>
+      </x:c>
+      <x:c r="D870" s="0" t="s">
+        <x:v>4114</x:v>
+      </x:c>
+      <x:c r="E870" s="0" t="s">
+        <x:v>4115</x:v>
+      </x:c>
+      <x:c r="F870" s="0" t="s">
+        <x:v>4116</x:v>
+      </x:c>
+      <x:c r="G870" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H870" s="1" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="I870" s="2" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="J870" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K870" s="3" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="L870" s="0" t="s"/>
+      <x:c r="M870" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N870" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O870" s="0" t="s"/>
+      <x:c r="P870" s="0" t="s"/>
+      <x:c r="Q870" s="0" t="s"/>
+      <x:c r="R870" s="0" t="s"/>
+      <x:c r="S870" s="0" t="s"/>
+      <x:c r="T870" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U870" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V870" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W870" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X870" s="0" t="s"/>
+      <x:c r="Y870" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z870" s="0" t="s"/>
+      <x:c r="AA870" s="0" t="s"/>
+      <x:c r="AB870" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC870" s="0" t="s"/>
+    </x:row>
+    <x:row r="871" spans="1:29">
+      <x:c r="A871" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B871" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C871" s="0" t="s">
+        <x:v>4117</x:v>
+      </x:c>
+      <x:c r="D871" s="0" t="s">
+        <x:v>4118</x:v>
+      </x:c>
+      <x:c r="E871" s="0" t="s">
+        <x:v>4119</x:v>
+      </x:c>
+      <x:c r="F871" s="0" t="s">
+        <x:v>4120</x:v>
+      </x:c>
+      <x:c r="G871" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H871" s="1" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I871" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="J871" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K871" s="3" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L871" s="0" t="s"/>
+      <x:c r="M871" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N871" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O871" s="0" t="s"/>
+      <x:c r="P871" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q871" s="0" t="s"/>
+      <x:c r="R871" s="0" t="s"/>
+      <x:c r="S871" s="0" t="s"/>
+      <x:c r="T871" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U871" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V871" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W871" s="0" t="s">
+        <x:v>4121</x:v>
+      </x:c>
+      <x:c r="X871" s="0" t="s"/>
+      <x:c r="Y871" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z871" s="0" t="s"/>
+      <x:c r="AA871" s="0" t="s"/>
+      <x:c r="AB871" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="AC871" s="0" t="s"/>
+    </x:row>
+    <x:row r="872" spans="1:29">
+      <x:c r="A872" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B872" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C872" s="0" t="s">
+        <x:v>4122</x:v>
+      </x:c>
+      <x:c r="D872" s="0" t="s">
+        <x:v>4123</x:v>
+      </x:c>
+      <x:c r="E872" s="0" t="s">
+        <x:v>4124</x:v>
+      </x:c>
+      <x:c r="F872" s="0" t="s">
+        <x:v>4125</x:v>
+      </x:c>
+      <x:c r="G872" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="H872" s="1" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="I872" s="2" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="J872" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K872" s="3" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="L872" s="0" t="s">
+        <x:v>4126</x:v>
+      </x:c>
+      <x:c r="M872" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N872" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O872" s="0" t="s"/>
+      <x:c r="P872" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q872" s="0" t="s">
+        <x:v>603</x:v>
+      </x:c>
+      <x:c r="R872" s="0" t="s">
+        <x:v>4127</x:v>
+      </x:c>
+      <x:c r="S872" s="0" t="s">
+        <x:v>3968</x:v>
+      </x:c>
+      <x:c r="T872" s="0" t="s">
+        <x:v>605</x:v>
+      </x:c>
+      <x:c r="U872" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V872" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="W872" s="0" t="s">
+        <x:v>1158</x:v>
+      </x:c>
+      <x:c r="X872" s="0" t="s"/>
+      <x:c r="Y872" s="0" t="s"/>
+      <x:c r="Z872" s="0" t="s"/>
+      <x:c r="AA872" s="0" t="s"/>
+      <x:c r="AB872" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC872" s="0" t="s"/>
+    </x:row>
+    <x:row r="873" spans="1:29">
+      <x:c r="A873" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B873" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C873" s="0" t="s">
+        <x:v>4128</x:v>
+      </x:c>
+      <x:c r="D873" s="0" t="s">
+        <x:v>4129</x:v>
+      </x:c>
+      <x:c r="E873" s="0" t="s">
+        <x:v>4130</x:v>
+      </x:c>
+      <x:c r="F873" s="0" t="s">
+        <x:v>4131</x:v>
+      </x:c>
+      <x:c r="G873" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="H873" s="1" t="s">
+        <x:v>4132</x:v>
+      </x:c>
+      <x:c r="I873" s="2" t="s">
+        <x:v>2719</x:v>
+      </x:c>
+      <x:c r="J873" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K873" s="3" t="s">
+        <x:v>2719</x:v>
+      </x:c>
+      <x:c r="L873" s="0" t="s">
+        <x:v>4133</x:v>
+      </x:c>
+      <x:c r="M873" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N873" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O873" s="0" t="s"/>
+      <x:c r="P873" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q873" s="0" t="s">
+        <x:v>4134</x:v>
+      </x:c>
+      <x:c r="R873" s="0" t="s">
+        <x:v>4135</x:v>
+      </x:c>
+      <x:c r="S873" s="0" t="s">
+        <x:v>3681</x:v>
+      </x:c>
+      <x:c r="T873" s="0" t="s">
+        <x:v>2469</x:v>
+      </x:c>
+      <x:c r="U873" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V873" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W873" s="0" t="s">
+        <x:v>3578</x:v>
+      </x:c>
+      <x:c r="X873" s="0" t="s"/>
+      <x:c r="Y873" s="0" t="s"/>
+      <x:c r="Z873" s="0" t="s"/>
+      <x:c r="AA873" s="0" t="s"/>
+      <x:c r="AB873" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC873" s="0" t="s"/>
+    </x:row>
+    <x:row r="874" spans="1:29">
+      <x:c r="A874" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B874" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C874" s="0" t="s">
+        <x:v>4136</x:v>
+      </x:c>
+      <x:c r="D874" s="0" t="s">
+        <x:v>4137</x:v>
+      </x:c>
+      <x:c r="E874" s="0" t="s">
+        <x:v>4138</x:v>
+      </x:c>
+      <x:c r="F874" s="0" t="s">
+        <x:v>4139</x:v>
+      </x:c>
+      <x:c r="G874" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H874" s="1" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="I874" s="2" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="J874" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K874" s="3" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="L874" s="0" t="s"/>
+      <x:c r="M874" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N874" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O874" s="0" t="s"/>
+      <x:c r="P874" s="0" t="s"/>
+      <x:c r="Q874" s="0" t="s"/>
+      <x:c r="R874" s="0" t="s"/>
+      <x:c r="S874" s="0" t="s"/>
+      <x:c r="T874" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U874" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V874" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W874" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="X874" s="0" t="s"/>
+      <x:c r="Y874" s="0" t="s">
+        <x:v>4140</x:v>
+      </x:c>
+      <x:c r="Z874" s="0" t="s"/>
+      <x:c r="AA874" s="0" t="s"/>
+      <x:c r="AB874" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC874" s="0" t="s"/>
+    </x:row>
+    <x:row r="875" spans="1:29">
+      <x:c r="A875" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B875" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C875" s="0" t="s">
+        <x:v>4128</x:v>
+      </x:c>
+      <x:c r="D875" s="0" t="s">
+        <x:v>4129</x:v>
+      </x:c>
+      <x:c r="E875" s="0" t="s">
+        <x:v>4130</x:v>
+      </x:c>
+      <x:c r="F875" s="0" t="s">
+        <x:v>4141</x:v>
+      </x:c>
+      <x:c r="G875" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H875" s="1" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="I875" s="2" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="J875" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K875" s="3" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="L875" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M875" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N875" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O875" s="0" t="s"/>
+      <x:c r="P875" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q875" s="0" t="s"/>
+      <x:c r="R875" s="0" t="s"/>
+      <x:c r="S875" s="0" t="s"/>
+      <x:c r="T875" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U875" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V875" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W875" s="0" t="s">
+        <x:v>3578</x:v>
+      </x:c>
+      <x:c r="X875" s="0" t="s"/>
+      <x:c r="Y875" s="0" t="s">
+        <x:v>4142</x:v>
+      </x:c>
+      <x:c r="Z875" s="0" t="s"/>
+      <x:c r="AA875" s="0" t="s"/>
+      <x:c r="AB875" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC875" s="0" t="s"/>
+    </x:row>
+    <x:row r="876" spans="1:29">
+      <x:c r="A876" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B876" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C876" s="0" t="s">
+        <x:v>4128</x:v>
+      </x:c>
+      <x:c r="D876" s="0" t="s">
+        <x:v>4129</x:v>
+      </x:c>
+      <x:c r="E876" s="0" t="s">
+        <x:v>4130</x:v>
+      </x:c>
+      <x:c r="F876" s="0" t="s">
+        <x:v>4143</x:v>
+      </x:c>
+      <x:c r="G876" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H876" s="1" t="s">
+        <x:v>898</x:v>
+      </x:c>
+      <x:c r="I876" s="2" t="s">
+        <x:v>898</x:v>
+      </x:c>
+      <x:c r="J876" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K876" s="3" t="s">
+        <x:v>898</x:v>
+      </x:c>
+      <x:c r="L876" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M876" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N876" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O876" s="0" t="s"/>
+      <x:c r="P876" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q876" s="0" t="s"/>
+      <x:c r="R876" s="0" t="s"/>
+      <x:c r="S876" s="0" t="s"/>
+      <x:c r="T876" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U876" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V876" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W876" s="0" t="s">
+        <x:v>3578</x:v>
+      </x:c>
+      <x:c r="X876" s="0" t="s"/>
+      <x:c r="Y876" s="0" t="s">
+        <x:v>4142</x:v>
+      </x:c>
+      <x:c r="Z876" s="0" t="s"/>
+      <x:c r="AA876" s="0" t="s"/>
+      <x:c r="AB876" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC876" s="0" t="s"/>
+    </x:row>
+    <x:row r="877" spans="1:29">
+      <x:c r="A877" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B877" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C877" s="0" t="s">
+        <x:v>4128</x:v>
+      </x:c>
+      <x:c r="D877" s="0" t="s">
+        <x:v>4129</x:v>
+      </x:c>
+      <x:c r="E877" s="0" t="s">
+        <x:v>4130</x:v>
+      </x:c>
+      <x:c r="F877" s="0" t="s">
+        <x:v>4144</x:v>
+      </x:c>
+      <x:c r="G877" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="H877" s="1" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I877" s="2" t="s">
+        <x:v>543</x:v>
+      </x:c>
+      <x:c r="J877" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K877" s="3" t="s">
+        <x:v>543</x:v>
+      </x:c>
+      <x:c r="L877" s="0" t="s">
+        <x:v>752</x:v>
+      </x:c>
+      <x:c r="M877" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N877" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="O877" s="0" t="s"/>
+      <x:c r="P877" s="0" t="s"/>
+      <x:c r="Q877" s="0" t="s"/>
+      <x:c r="R877" s="0" t="s">
+        <x:v>4145</x:v>
+      </x:c>
+      <x:c r="S877" s="0" t="s"/>
+      <x:c r="T877" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="U877" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V877" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W877" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X877" s="0" t="s"/>
+      <x:c r="Y877" s="0" t="s"/>
+      <x:c r="Z877" s="0" t="s"/>
+      <x:c r="AA877" s="0" t="s"/>
+      <x:c r="AB877" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC877" s="0" t="s"/>
+    </x:row>
+    <x:row r="878" spans="1:29">
+      <x:c r="A878" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B878" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C878" s="0" t="s">
+        <x:v>4146</x:v>
+      </x:c>
+      <x:c r="D878" s="0" t="s">
+        <x:v>4147</x:v>
+      </x:c>
+      <x:c r="E878" s="0" t="s">
+        <x:v>4148</x:v>
+      </x:c>
+      <x:c r="F878" s="0" t="s">
+        <x:v>4149</x:v>
+      </x:c>
+      <x:c r="G878" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="H878" s="1" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="I878" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J878" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K878" s="3" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="L878" s="0" t="s"/>
+      <x:c r="M878" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N878" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O878" s="0" t="s"/>
+      <x:c r="P878" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="Q878" s="0" t="s"/>
+      <x:c r="R878" s="0" t="s"/>
+      <x:c r="S878" s="0" t="s"/>
+      <x:c r="T878" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="U878" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V878" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W878" s="0" t="s">
+        <x:v>4150</x:v>
+      </x:c>
+      <x:c r="X878" s="0" t="s"/>
+      <x:c r="Y878" s="0" t="s">
+        <x:v>4151</x:v>
+      </x:c>
+      <x:c r="Z878" s="0" t="s"/>
+      <x:c r="AA878" s="0" t="s"/>
+      <x:c r="AB878" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC878" s="0" t="s"/>
+    </x:row>
+    <x:row r="879" spans="1:29">
+      <x:c r="A879" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B879" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C879" s="0" t="s">
+        <x:v>4152</x:v>
+      </x:c>
+      <x:c r="D879" s="0" t="s">
+        <x:v>4153</x:v>
+      </x:c>
+      <x:c r="E879" s="0" t="s">
+        <x:v>4154</x:v>
+      </x:c>
+      <x:c r="F879" s="0" t="s">
+        <x:v>4155</x:v>
+      </x:c>
+      <x:c r="G879" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="H879" s="1" t="s">
+        <x:v>913</x:v>
+      </x:c>
+      <x:c r="I879" s="2" t="s">
+        <x:v>913</x:v>
+      </x:c>
+      <x:c r="J879" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K879" s="3" t="s">
+        <x:v>913</x:v>
+      </x:c>
+      <x:c r="L879" s="0" t="s">
+        <x:v>4156</x:v>
+      </x:c>
+      <x:c r="M879" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N879" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O879" s="0" t="s"/>
+      <x:c r="P879" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q879" s="0" t="s"/>
+      <x:c r="R879" s="0" t="s">
+        <x:v>4157</x:v>
+      </x:c>
+      <x:c r="S879" s="0" t="s"/>
+      <x:c r="T879" s="0" t="s">
+        <x:v>3911</x:v>
+      </x:c>
+      <x:c r="U879" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V879" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W879" s="0" t="s">
+        <x:v>720</x:v>
+      </x:c>
+      <x:c r="X879" s="0" t="s"/>
+      <x:c r="Y879" s="0" t="s"/>
+      <x:c r="Z879" s="0" t="s"/>
+      <x:c r="AA879" s="0" t="s"/>
+      <x:c r="AB879" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC879" s="0" t="s"/>
+    </x:row>
+    <x:row r="880" spans="1:29">
+      <x:c r="A880" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B880" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C880" s="0" t="s">
+        <x:v>4158</x:v>
+      </x:c>
+      <x:c r="D880" s="0" t="s">
+        <x:v>4159</x:v>
+      </x:c>
+      <x:c r="E880" s="0" t="s">
+        <x:v>4160</x:v>
+      </x:c>
+      <x:c r="F880" s="0" t="s">
+        <x:v>4161</x:v>
+      </x:c>
+      <x:c r="G880" s="0" t="s">
+        <x:v>4162</x:v>
+      </x:c>
+      <x:c r="H880" s="1" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="I880" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J880" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K880" s="3" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="L880" s="0" t="s"/>
+      <x:c r="M880" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N880" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O880" s="0" t="s"/>
+      <x:c r="P880" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q880" s="0" t="s"/>
+      <x:c r="R880" s="0" t="s"/>
+      <x:c r="S880" s="0" t="s"/>
+      <x:c r="T880" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U880" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V880" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W880" s="0" t="s">
+        <x:v>515</x:v>
+      </x:c>
+      <x:c r="X880" s="0" t="s"/>
+      <x:c r="Y880" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z880" s="0" t="s"/>
+      <x:c r="AA880" s="0" t="s"/>
+      <x:c r="AB880" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC880" s="0" t="s"/>
+    </x:row>
+    <x:row r="881" spans="1:29">
+      <x:c r="A881" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B881" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C881" s="0" t="s">
+        <x:v>3377</x:v>
+      </x:c>
+      <x:c r="D881" s="0" t="s">
+        <x:v>3378</x:v>
+      </x:c>
+      <x:c r="E881" s="0" t="s">
+        <x:v>3379</x:v>
+      </x:c>
+      <x:c r="F881" s="0" t="s">
+        <x:v>4163</x:v>
+      </x:c>
+      <x:c r="G881" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H881" s="1" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="I881" s="2" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="J881" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K881" s="3" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="L881" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M881" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N881" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O881" s="0" t="s"/>
+      <x:c r="P881" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Q881" s="0" t="s"/>
+      <x:c r="R881" s="0" t="s"/>
+      <x:c r="S881" s="0" t="s"/>
+      <x:c r="T881" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="U881" s="0" t="s">
+        <x:v>414</x:v>
+      </x:c>
+      <x:c r="V881" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="W881" s="0" t="s">
+        <x:v>1334</x:v>
+      </x:c>
+      <x:c r="X881" s="0" t="s"/>
+      <x:c r="Y881" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Z881" s="0" t="s"/>
+      <x:c r="AA881" s="0" t="s"/>
+      <x:c r="AB881" s="0" t="s">
+        <x:v>3384</x:v>
+      </x:c>
+      <x:c r="AC881" s="0" t="s"/>
+    </x:row>
+    <x:row r="882" spans="1:29">
+      <x:c r="A882" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B882" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C882" s="0" t="s">
+        <x:v>4164</x:v>
+      </x:c>
+      <x:c r="D882" s="0" t="s">
+        <x:v>4165</x:v>
+      </x:c>
+      <x:c r="E882" s="0" t="s">
+        <x:v>4166</x:v>
+      </x:c>
+      <x:c r="F882" s="0" t="s">
+        <x:v>4167</x:v>
+      </x:c>
+      <x:c r="G882" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="H882" s="1" t="s">
+        <x:v>4168</x:v>
+      </x:c>
+      <x:c r="I882" s="2" t="s">
+        <x:v>4168</x:v>
+      </x:c>
+      <x:c r="J882" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K882" s="3" t="s">
+        <x:v>4168</x:v>
+      </x:c>
+      <x:c r="L882" s="0" t="s">
+        <x:v>4169</x:v>
+      </x:c>
+      <x:c r="M882" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N882" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O882" s="0" t="s"/>
+      <x:c r="P882" s="0" t="s"/>
+      <x:c r="Q882" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="R882" s="0" t="s">
+        <x:v>4170</x:v>
+      </x:c>
+      <x:c r="S882" s="0" t="s">
+        <x:v>3968</x:v>
+      </x:c>
+      <x:c r="T882" s="0" t="s">
+        <x:v>2469</x:v>
+      </x:c>
+      <x:c r="U882" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="V882" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="W882" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X882" s="0" t="s"/>
+      <x:c r="Y882" s="0" t="s"/>
+      <x:c r="Z882" s="0" t="s"/>
+      <x:c r="AA882" s="0" t="s"/>
+      <x:c r="AB882" s="0" t="s">
+        <x:v>4171</x:v>
+      </x:c>
+      <x:c r="AC882" s="0" t="s"/>
+    </x:row>
+    <x:row r="883" spans="1:29">
+      <x:c r="A883" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B883" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C883" s="0" t="s">
+        <x:v>4172</x:v>
+      </x:c>
+      <x:c r="D883" s="0" t="s">
+        <x:v>4173</x:v>
+      </x:c>
+      <x:c r="E883" s="0" t="s">
+        <x:v>4174</x:v>
+      </x:c>
+      <x:c r="F883" s="0" t="s">
+        <x:v>4175</x:v>
+      </x:c>
+      <x:c r="G883" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H883" s="1" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="I883" s="2" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="J883" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K883" s="3" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="L883" s="0" t="s"/>
+      <x:c r="M883" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N883" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O883" s="0" t="s"/>
+      <x:c r="P883" s="0" t="s"/>
+      <x:c r="Q883" s="0" t="s"/>
+      <x:c r="R883" s="0" t="s"/>
+      <x:c r="S883" s="0" t="s"/>
+      <x:c r="T883" s="0" t="s">
+        <x:v>3806</x:v>
+      </x:c>
+      <x:c r="U883" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="V883" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="W883" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X883" s="0" t="s"/>
+      <x:c r="Y883" s="0" t="s">
+        <x:v>3853</x:v>
+      </x:c>
+      <x:c r="Z883" s="0" t="s"/>
+      <x:c r="AA883" s="0" t="s"/>
+      <x:c r="AB883" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="AC883" s="0" t="s"/>
+    </x:row>
+    <x:row r="884" spans="1:29">
+      <x:c r="A884" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="B884" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C884" s="0" t="s">
+        <x:v>4176</x:v>
+      </x:c>
+      <x:c r="D884" s="0" t="s">
+        <x:v>4177</x:v>
+      </x:c>
+      <x:c r="E884" s="0" t="s">
+        <x:v>4178</x:v>
+      </x:c>
+      <x:c r="F884" s="0" t="s">
+        <x:v>4179</x:v>
+      </x:c>
+      <x:c r="G884" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H884" s="1" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I884" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="J884" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K884" s="3" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="L884" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M884" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N884" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="O884" s="0" t="s"/>
+      <x:c r="P884" s="0" t="s"/>
+      <x:c r="Q884" s="0" t="s"/>
+      <x:c r="R884" s="0" t="s"/>
+      <x:c r="S884" s="0" t="s"/>
+      <x:c r="T884" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="U884" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V884" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="W884" s="0" t="s">
+        <x:v>1941</x:v>
+      </x:c>
+      <x:c r="X884" s="0" t="s"/>
+      <x:c r="Y884" s="0" t="s">
+        <x:v>4180</x:v>
+      </x:c>
+      <x:c r="Z884" s="0" t="s"/>
+      <x:c r="AA884" s="0" t="s"/>
+      <x:c r="AB884" s="0" t="s"/>
+      <x:c r="AC884" s="0" t="s"/>
+    </x:row>
+    <x:row r="885" spans="1:29">
+      <x:c r="A885" s="0" t="s"/>
+      <x:c r="B885" s="0" t="s"/>
+      <x:c r="C885" s="0" t="s"/>
+      <x:c r="D885" s="0" t="s"/>
+      <x:c r="E885" s="0" t="s"/>
+      <x:c r="F885" s="0" t="s"/>
+      <x:c r="G885" s="0" t="s"/>
+      <x:c r="H885" s="0" t="s"/>
+      <x:c r="I885" s="0" t="s"/>
+      <x:c r="J885" s="0" t="s"/>
+      <x:c r="K885" s="0" t="s"/>
+      <x:c r="L885" s="0" t="s"/>
+      <x:c r="M885" s="0" t="s"/>
+      <x:c r="N885" s="0" t="s"/>
+      <x:c r="O885" s="0" t="s"/>
+      <x:c r="P885" s="0" t="s"/>
+      <x:c r="Q885" s="0" t="s"/>
+      <x:c r="R885" s="0" t="s"/>
+      <x:c r="S885" s="0" t="s"/>
+      <x:c r="T885" s="0" t="s"/>
+      <x:c r="U885" s="0" t="s"/>
+      <x:c r="V885" s="0" t="s"/>
+      <x:c r="W885" s="0" t="s"/>
+      <x:c r="X885" s="0" t="s"/>
+      <x:c r="Y885" s="0" t="s"/>
+      <x:c r="Z885" s="0" t="s"/>
+      <x:c r="AA885" s="0" t="s"/>
+      <x:c r="AB885" s="0" t="s"/>
+      <x:c r="AC885" s="0" t="s"/>
+    </x:row>
+    <x:row r="886" spans="1:29">
+      <x:c r="A886" s="0" t="s"/>
+      <x:c r="B886" s="0" t="s"/>
+      <x:c r="C886" s="0" t="s"/>
+      <x:c r="D886" s="0" t="s">
+        <x:v>4181</x:v>
+      </x:c>
+      <x:c r="E886" s="0" t="s"/>
+      <x:c r="F886" s="0" t="s"/>
+      <x:c r="G886" s="0" t="s"/>
+      <x:c r="H886" s="0" t="s">
+        <x:v>4182</x:v>
+      </x:c>
+      <x:c r="I886" s="0" t="s">
+        <x:v>4183</x:v>
+      </x:c>
+      <x:c r="J886" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K886" s="0" t="s"/>
+      <x:c r="L886" s="0" t="s">
+        <x:v>4184</x:v>
+      </x:c>
+      <x:c r="M886" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="N886" s="0" t="s">
+        <x:v>4185</x:v>
+      </x:c>
+      <x:c r="O886" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="P886" s="0" t="s">
+        <x:v>4186</x:v>
+      </x:c>
+      <x:c r="Q886" s="0" t="s"/>
+      <x:c r="R886" s="0" t="s"/>
+      <x:c r="S886" s="0" t="s"/>
+      <x:c r="T886" s="0" t="s"/>
+      <x:c r="U886" s="0" t="s"/>
+      <x:c r="V886" s="0" t="s"/>
+      <x:c r="W886" s="0" t="s"/>
+      <x:c r="X886" s="0" t="s"/>
+      <x:c r="Y886" s="0" t="s"/>
+      <x:c r="Z886" s="0" t="s"/>
+      <x:c r="AA886" s="0" t="s"/>
+      <x:c r="AB886" s="0" t="s"/>
+      <x:c r="AC886" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>